<commit_message>
remoção z-lacunas da pasta Monitoramento
</commit_message>
<xml_diff>
--- a/scripts/Monitoramento/inputs/0 - Expansão MS/0 - Monitoramento Form 4.xlsx
+++ b/scripts/Monitoramento/inputs/0 - Expansão MS/0 - Monitoramento Form 4.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29602"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29609"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_60946DCC6662C8E28B6EBEE7554C260622F1E00E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0ADDEB3F-DCC5-4B3A-977C-E35C874C9EAE}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_715C6DCC381206EEB8FD79FE63CDA88F4A77FA50" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C23AB675-7E21-463F-90C3-F506D2AB01A0}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="10" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumo" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3395" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3405" uniqueCount="192">
   <si>
     <t>Categoria</t>
   </si>
@@ -540,6 +540,9 @@
     <t>08/10/2025</t>
   </si>
   <si>
+    <t>10/12/2025</t>
+  </si>
+  <si>
     <t>26/09/2025</t>
   </si>
   <si>
@@ -600,6 +603,9 @@
     <t>17/11/2025</t>
   </si>
   <si>
+    <t>09/12/2025</t>
+  </si>
+  <si>
     <t>13/11/2025</t>
   </si>
   <si>
@@ -612,13 +618,19 @@
     <t>02/12/2025</t>
   </si>
   <si>
+    <t>15/12/2025</t>
+  </si>
+  <si>
     <t>08/12/2025</t>
   </si>
   <si>
     <t>04/12/2025</t>
   </si>
   <si>
-    <t>09/12/2025</t>
+    <t>12/12/2025</t>
+  </si>
+  <si>
+    <t>11/12/2025</t>
   </si>
   <si>
     <t>Mês de referência</t>
@@ -876,14 +888,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF66FF66"/>
-        <bgColor rgb="FF66FF66"/>
+        <fgColor rgb="FF008000"/>
+        <bgColor rgb="FF008000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF008000"/>
-        <bgColor rgb="FF008000"/>
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF808080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FF66"/>
+        <bgColor rgb="FF66FF66"/>
       </patternFill>
     </fill>
     <fill>
@@ -912,20 +930,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF808080"/>
+        <fgColor rgb="FF006400"/>
+        <bgColor rgb="FF006400"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF6666"/>
         <bgColor rgb="FFFF6666"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF006400"/>
-        <bgColor rgb="FF006400"/>
       </patternFill>
     </fill>
     <fill>
@@ -1226,16 +1238,13 @@
     <xf numFmtId="0" fontId="17" fillId="23" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="26" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1250,19 +1259,22 @@
     <xf numFmtId="0" fontId="15" fillId="29" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1376,9 +1388,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1406,11 +1415,17 @@
     <xf numFmtId="0" fontId="7" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1421,15 +1436,6 @@
     <xf numFmtId="0" fontId="4" fillId="17" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="11" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1437,6 +1443,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="11" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -3484,7 +3496,7 @@
       </c>
       <c r="I2" s="54">
         <f ca="1">COUNTIF(INDIRECT(I$1&amp;"!E2:E1000"),$A2)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J2" s="54">
         <f ca="1">COUNTIF(INDIRECT(J$1&amp;"!E2:E1000"),$A2)</f>
@@ -3492,11 +3504,11 @@
       </c>
       <c r="K2" s="54">
         <f ca="1">COUNTIF(INDIRECT(K$1&amp;"!E2:E1000"),$A2)</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="L2" s="54">
         <f ca="1">COUNTIF(INDIRECT(L$1&amp;"!E2:E1000"),$A2)</f>
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="M2" s="54">
         <f ca="1">COUNTIF(INDIRECT(M$1&amp;"!E2:E1000"),$A2)</f>
@@ -3504,7 +3516,7 @@
       </c>
       <c r="N2" s="55">
         <f ca="1">SUM(B2:M2)</f>
-        <v>65</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1">
@@ -3553,7 +3565,7 @@
       </c>
       <c r="L3" s="56">
         <f ca="1">COUNTIF(INDIRECT(L$1&amp;"!E2:E1000"),$A3)</f>
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="M3" s="56">
         <f ca="1">COUNTIF(INDIRECT(M$1&amp;"!E2:E1000"),$A3)</f>
@@ -3561,7 +3573,7 @@
       </c>
       <c r="N3" s="57">
         <f ca="1">SUM(B3:M3)</f>
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1">
@@ -3598,7 +3610,7 @@
       </c>
       <c r="I4" s="58">
         <f ca="1">COUNTIF(INDIRECT(I$1&amp;"!E2:E1000"),$A4)</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J4" s="58">
         <f ca="1">COUNTIF(INDIRECT(J$1&amp;"!E2:E1000"),$A4)</f>
@@ -3606,7 +3618,7 @@
       </c>
       <c r="K4" s="58">
         <f ca="1">COUNTIF(INDIRECT(K$1&amp;"!E2:E1000"),$A4)</f>
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L4" s="58">
         <f ca="1">COUNTIF(INDIRECT(L$1&amp;"!E2:E1000"),$A4)</f>
@@ -3618,7 +3630,7 @@
       </c>
       <c r="N4" s="59">
         <f ca="1">SUM(B4:M4)</f>
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1">
@@ -3891,11 +3903,11 @@
       <c r="U10" s="12"/>
     </row>
     <row r="11" spans="1:21" ht="21" customHeight="1">
-      <c r="A11" s="99" t="s">
+      <c r="A11" s="107" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="109"/>
-      <c r="C11" s="97" t="s">
+      <c r="C11" s="96" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="110"/>
@@ -3905,7 +3917,7 @@
       <c r="H11" s="110"/>
       <c r="I11" s="109"/>
       <c r="J11" s="12"/>
-      <c r="K11" s="97" t="s">
+      <c r="K11" s="96" t="s">
         <v>22</v>
       </c>
       <c r="L11" s="110"/>
@@ -3914,7 +3926,7 @@
       <c r="O11" s="110"/>
       <c r="P11" s="109"/>
       <c r="Q11" s="13"/>
-      <c r="R11" s="89" t="s">
+      <c r="R11" s="88" t="s">
         <v>23</v>
       </c>
       <c r="S11" s="110"/>
@@ -3922,11 +3934,11 @@
       <c r="U11" s="12"/>
     </row>
     <row r="12" spans="1:21" ht="15" customHeight="1">
-      <c r="A12" s="103" t="s">
+      <c r="A12" s="108" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="111"/>
-      <c r="C12" s="96" t="s">
+      <c r="C12" s="95" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="110"/>
@@ -3936,7 +3948,7 @@
       <c r="H12" s="110"/>
       <c r="I12" s="109"/>
       <c r="J12" s="12"/>
-      <c r="K12" s="96" t="s">
+      <c r="K12" s="95" t="s">
         <v>24</v>
       </c>
       <c r="L12" s="110"/>
@@ -3945,7 +3957,7 @@
       <c r="O12" s="110"/>
       <c r="P12" s="109"/>
       <c r="Q12" s="13"/>
-      <c r="R12" s="88" t="s">
+      <c r="R12" s="100" t="s">
         <v>25</v>
       </c>
       <c r="S12" s="109"/>
@@ -3998,7 +4010,7 @@
         <v>32</v>
       </c>
       <c r="Q13" s="13"/>
-      <c r="R13" s="95" t="str">
+      <c r="R13" s="94" t="str">
         <f>_xlfn.CONCAT("Envios - Mês de Referência - ", A12)</f>
         <v>Envios - Mês de Referência - 08.25</v>
       </c>
@@ -4039,11 +4051,11 @@
       <c r="J14" s="17"/>
       <c r="K14" s="71">
         <f ca="1">COUNTIF(INDIRECT("Monitoramento!$D$2:$Q$15"), "Enviado")</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L14" s="56">
         <f ca="1">COUNTIF(INDIRECT("Monitoramento!$D$2:$Q$15"), "Atrasado")</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M14" s="58">
         <f ca="1">COUNTIF(INDIRECT("Monitoramento!$D$2:$Q$15"), "Atrasado &gt;= 2")</f>
@@ -4083,7 +4095,7 @@
       </c>
       <c r="D15" s="70">
         <f t="array" aca="1" ref="D15" ca="1">IFERROR(ROWS(_xlfn._xlws.FILTER(INDIRECT($A$12&amp;"!A2:E100"),(INDIRECT($A$12&amp;"!A2:A100")=$C15)*(INDIRECT($A$12&amp;"!E2:E100")="Enviado"))), 0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E15" s="56">
         <f t="array" aca="1" ref="E15" ca="1">IFERROR(ROWS(_xlfn._xlws.FILTER(INDIRECT($A$12&amp;"!A2:E100"),(INDIRECT($A$12&amp;"!A2:A100")=$C15)*(INDIRECT($A$12&amp;"!E2:E100")="Atrasado"))), 0)</f>
@@ -4091,7 +4103,7 @@
       </c>
       <c r="F15" s="58">
         <f t="array" aca="1" ref="F15" ca="1">IFERROR(ROWS(_xlfn._xlws.FILTER(INDIRECT($A$12&amp;"!A2:E100"),(INDIRECT($A$12&amp;"!A2:A100")=$C15)*(INDIRECT($A$12&amp;"!E2:E100")="Atrasado &gt;= 2"))), 0)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G15" s="60">
         <f t="array" aca="1" ref="G15" ca="1">IFERROR(ROWS(_xlfn._xlws.FILTER(INDIRECT($A$12&amp;"!A2:E100"),(INDIRECT($A$12&amp;"!A2:A100")=$C15)*(INDIRECT($A$12&amp;"!E2:E100")="Duplicado"))), 0)</f>
@@ -4108,15 +4120,15 @@
       <c r="J15" s="16"/>
       <c r="K15" s="71">
         <f ca="1">COUNTIF(INDIRECT("Monitoramento!$D$18:$Q$31"), "Enviado")</f>
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="L15" s="56">
         <f ca="1">COUNTIF(INDIRECT("Monitoramento!$D$18:$Q$31"), "Atrasado")</f>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M15" s="58">
         <f ca="1">COUNTIF(INDIRECT("Monitoramento!$D$18:$Q$31"), "Atrasado &gt;= 2")</f>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="N15" s="60">
         <f ca="1">COUNTIF(INDIRECT("Monitoramento!$D$18:$Q$31"), "Duplicado")</f>
@@ -4354,7 +4366,7 @@
     <row r="19" spans="1:21" ht="15" customHeight="1">
       <c r="A19" s="112"/>
       <c r="B19" s="113"/>
-      <c r="C19" s="96" t="s">
+      <c r="C19" s="95" t="s">
         <v>41</v>
       </c>
       <c r="D19" s="110"/>
@@ -4364,7 +4376,7 @@
       <c r="H19" s="110"/>
       <c r="I19" s="109"/>
       <c r="J19" s="26"/>
-      <c r="K19" s="96" t="s">
+      <c r="K19" s="95" t="s">
         <v>41</v>
       </c>
       <c r="L19" s="110"/>
@@ -4389,15 +4401,15 @@
     <row r="20" spans="1:21" ht="15" customHeight="1">
       <c r="A20" s="112"/>
       <c r="B20" s="113"/>
-      <c r="C20" s="88" t="s">
+      <c r="C20" s="100" t="s">
         <v>25</v>
       </c>
       <c r="D20" s="109"/>
-      <c r="E20" s="88" t="s">
+      <c r="E20" s="100" t="s">
         <v>42</v>
       </c>
       <c r="F20" s="109"/>
-      <c r="G20" s="88" t="s">
+      <c r="G20" s="100" t="s">
         <v>43</v>
       </c>
       <c r="H20" s="109"/>
@@ -4405,15 +4417,15 @@
         <v>44</v>
       </c>
       <c r="J20" s="17"/>
-      <c r="K20" s="101" t="s">
+      <c r="K20" s="102" t="s">
         <v>42</v>
       </c>
       <c r="L20" s="114"/>
-      <c r="M20" s="101" t="s">
+      <c r="M20" s="102" t="s">
         <v>43</v>
       </c>
       <c r="N20" s="114"/>
-      <c r="O20" s="101" t="s">
+      <c r="O20" s="102" t="s">
         <v>45</v>
       </c>
       <c r="P20" s="114"/>
@@ -4421,7 +4433,7 @@
       <c r="R20" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="S20" s="92">
+      <c r="S20" s="91">
         <f ca="1">VLOOKUP($T$12,$C$21:$I$25,7,FALSE)</f>
         <v>0</v>
       </c>
@@ -4431,16 +4443,16 @@
     <row r="21" spans="1:21" ht="15" customHeight="1">
       <c r="A21" s="112"/>
       <c r="B21" s="113"/>
-      <c r="C21" s="107" t="s">
+      <c r="C21" s="105" t="s">
         <v>33</v>
       </c>
       <c r="D21" s="109"/>
-      <c r="E21" s="90">
+      <c r="E21" s="89">
         <f t="array" aca="1" ref="E21" ca="1">IFERROR(ROWS(_xlfn._xlws.FILTER(INDIRECT($A$12&amp;"!A2:E100"),(INDIRECT($A$12&amp;"!A2:A100")=$C21)*(INDIRECT($A$12&amp;"!G2:G100")="Sim"))), 0)</f>
         <v>0</v>
       </c>
       <c r="F21" s="109"/>
-      <c r="G21" s="91">
+      <c r="G21" s="90">
         <f t="array" aca="1" ref="G21" ca="1">IFERROR(ROWS(_xlfn._xlws.FILTER(INDIRECT($A$12&amp;"!A2:E100"),(INDIRECT($A$12&amp;"!A2:A100")=$C21)*(INDIRECT($A$12&amp;"!G2:G100")="Não"))), 0)</f>
         <v>8</v>
       </c>
@@ -4450,23 +4462,23 @@
         <v>0</v>
       </c>
       <c r="J21" s="16"/>
-      <c r="K21" s="90">
+      <c r="K21" s="89">
         <f ca="1">COUNTIF(INDIRECT("Regionais!D2:Q15"), "Sim")</f>
         <v>84</v>
       </c>
       <c r="L21" s="109"/>
-      <c r="M21" s="91">
+      <c r="M21" s="90">
         <f ca="1">COUNTIF(INDIRECT("Regionais!D2:Q15"), "Não")</f>
         <v>49</v>
       </c>
       <c r="N21" s="109"/>
-      <c r="O21" s="94">
+      <c r="O21" s="93">
         <f ca="1">IFERROR(K21/SUM(K21:N21), 0)</f>
         <v>0.63157894736842102</v>
       </c>
       <c r="P21" s="109"/>
       <c r="Q21" s="13"/>
-      <c r="R21" s="95" t="s">
+      <c r="R21" s="94" t="s">
         <v>47</v>
       </c>
       <c r="S21" s="110"/>
@@ -4476,16 +4488,16 @@
     <row r="22" spans="1:21" ht="15" customHeight="1">
       <c r="A22" s="112"/>
       <c r="B22" s="113"/>
-      <c r="C22" s="102" t="s">
+      <c r="C22" s="103" t="s">
         <v>35</v>
       </c>
       <c r="D22" s="109"/>
-      <c r="E22" s="90">
+      <c r="E22" s="89">
         <f t="array" aca="1" ref="E22" ca="1">IFERROR(ROWS(_xlfn._xlws.FILTER(INDIRECT($A$12&amp;"!A2:E100"),(INDIRECT($A$12&amp;"!A2:A100")=$C22)*(INDIRECT($A$12&amp;"!G2:G100")="Sim"))), 0)</f>
         <v>0</v>
       </c>
       <c r="F22" s="109"/>
-      <c r="G22" s="91">
+      <c r="G22" s="90">
         <f t="array" aca="1" ref="G22" ca="1">IFERROR(ROWS(_xlfn._xlws.FILTER(INDIRECT($A$12&amp;"!A2:E100"),(INDIRECT($A$12&amp;"!A2:A100")=$C22)*(INDIRECT($A$12&amp;"!G2:G100")="Não"))), 0)</f>
         <v>11</v>
       </c>
@@ -4495,17 +4507,17 @@
         <v>0</v>
       </c>
       <c r="J22" s="17"/>
-      <c r="K22" s="90">
+      <c r="K22" s="89">
         <f ca="1">COUNTIF(INDIRECT("Regionais!D18:Q31"), "Sim")</f>
         <v>84</v>
       </c>
       <c r="L22" s="109"/>
-      <c r="M22" s="91">
+      <c r="M22" s="90">
         <f ca="1">COUNTIF(INDIRECT("Regionais!D18:Q31"), "Não")</f>
         <v>49</v>
       </c>
       <c r="N22" s="109"/>
-      <c r="O22" s="94">
+      <c r="O22" s="93">
         <f ca="1">IFERROR(K22/SUM(K22:N22), 0)</f>
         <v>0.63157894736842102</v>
       </c>
@@ -4527,16 +4539,16 @@
     <row r="23" spans="1:21" ht="15" customHeight="1">
       <c r="A23" s="112"/>
       <c r="B23" s="113"/>
-      <c r="C23" s="108" t="s">
+      <c r="C23" s="106" t="s">
         <v>37</v>
       </c>
       <c r="D23" s="109"/>
-      <c r="E23" s="90">
+      <c r="E23" s="89">
         <f t="array" aca="1" ref="E23" ca="1">IFERROR(ROWS(_xlfn._xlws.FILTER(INDIRECT($A$12&amp;"!A2:E100"),(INDIRECT($A$12&amp;"!A2:A100")=$C23)*(INDIRECT($A$12&amp;"!G2:G100")="Sim"))), 0)</f>
         <v>1</v>
       </c>
       <c r="F23" s="109"/>
-      <c r="G23" s="100">
+      <c r="G23" s="101">
         <f t="array" aca="1" ref="G23" ca="1">IFERROR(ROWS(_xlfn._xlws.FILTER(INDIRECT($A$12&amp;"!A2:E100"),(INDIRECT($A$12&amp;"!A2:A100")=$C23)*(INDIRECT($A$12&amp;"!G2:G100")="Não"))), 0)</f>
         <v>9</v>
       </c>
@@ -4546,17 +4558,17 @@
         <v>0.1</v>
       </c>
       <c r="J23" s="17"/>
-      <c r="K23" s="90">
+      <c r="K23" s="89">
         <f ca="1">COUNTIF(INDIRECT("Regionais!D34:Q47"), "Sim")</f>
         <v>70</v>
       </c>
       <c r="L23" s="109"/>
-      <c r="M23" s="91">
+      <c r="M23" s="90">
         <f ca="1">COUNTIF(INDIRECT("Regionais!D34:Q47"), "Não")</f>
         <v>44</v>
       </c>
       <c r="N23" s="109"/>
-      <c r="O23" s="94">
+      <c r="O23" s="93">
         <f ca="1">IFERROR(K23/SUM(K23:N23), 0)</f>
         <v>0.61403508771929827</v>
       </c>
@@ -4578,16 +4590,16 @@
     <row r="24" spans="1:21" ht="15" customHeight="1">
       <c r="A24" s="112"/>
       <c r="B24" s="113"/>
-      <c r="C24" s="104" t="s">
+      <c r="C24" s="97" t="s">
         <v>39</v>
       </c>
       <c r="D24" s="109"/>
-      <c r="E24" s="105">
+      <c r="E24" s="98">
         <f t="array" aca="1" ref="E24" ca="1">IFERROR(ROWS(_xlfn._xlws.FILTER(INDIRECT($A$12&amp;"!A2:E100"),(INDIRECT($A$12&amp;"!A2:A100")=$C24)*(INDIRECT($A$12&amp;"!G2:G100")="Sim"))), 0)</f>
         <v>0</v>
       </c>
       <c r="F24" s="110"/>
-      <c r="G24" s="91">
+      <c r="G24" s="90">
         <f t="array" aca="1" ref="G24" ca="1">IFERROR(ROWS(_xlfn._xlws.FILTER(INDIRECT($A$12&amp;"!A2:E100"),(INDIRECT($A$12&amp;"!A2:A100")=$C24)*(INDIRECT($A$12&amp;"!G2:G100")="Não"))), 0)</f>
         <v>4</v>
       </c>
@@ -4597,17 +4609,17 @@
         <v>0</v>
       </c>
       <c r="J24" s="12"/>
-      <c r="K24" s="90">
+      <c r="K24" s="89">
         <f ca="1">COUNTIF(INDIRECT("Regionais!D50:Q63"), "Sim")</f>
         <v>41</v>
       </c>
       <c r="L24" s="109"/>
-      <c r="M24" s="91">
+      <c r="M24" s="90">
         <f ca="1">COUNTIF(INDIRECT("Regionais!D50:Q63"), "Não")</f>
         <v>26</v>
       </c>
       <c r="N24" s="109"/>
-      <c r="O24" s="94">
+      <c r="O24" s="93">
         <f ca="1">IFERROR(K24/SUM(K24:N24), 0)</f>
         <v>0.61194029850746268</v>
       </c>
@@ -4629,16 +4641,16 @@
     <row r="25" spans="1:21">
       <c r="A25" s="112"/>
       <c r="B25" s="113"/>
-      <c r="C25" s="106" t="s">
+      <c r="C25" s="104" t="s">
         <v>26</v>
       </c>
       <c r="D25" s="109"/>
-      <c r="E25" s="90">
+      <c r="E25" s="89">
         <f t="array" aca="1" ref="E25" ca="1">IFERROR(ROWS(_xlfn._xlws.FILTER(INDIRECT($A$12&amp;"!A2:E100"),(INDIRECT($A$12&amp;"!A2:A100")=$C25)*(INDIRECT($A$12&amp;"!G2:G100")="Sim"))), 0)</f>
         <v>0</v>
       </c>
       <c r="F25" s="109"/>
-      <c r="G25" s="93">
+      <c r="G25" s="92">
         <f t="array" aca="1" ref="G25" ca="1">IFERROR(ROWS(_xlfn._xlws.FILTER(INDIRECT($A$12&amp;"!A2:E100"),(INDIRECT($A$12&amp;"!A2:A100")=$C25)*(INDIRECT($A$12&amp;"!G2:G100")="Não"))), 0)</f>
         <v>13</v>
       </c>
@@ -4648,17 +4660,17 @@
         <v>0</v>
       </c>
       <c r="J25" s="12"/>
-      <c r="K25" s="90">
+      <c r="K25" s="89">
         <f ca="1">COUNTIF(INDIRECT("Regionais!D66:Q78"), "Sim")</f>
         <v>0</v>
       </c>
       <c r="L25" s="109"/>
-      <c r="M25" s="91">
+      <c r="M25" s="90">
         <f ca="1">COUNTIF(INDIRECT("Regionais!D66:Q78"), "Não")</f>
         <v>0</v>
       </c>
       <c r="N25" s="109"/>
-      <c r="O25" s="94">
+      <c r="O25" s="93">
         <f ca="1">IFERROR(K25/SUM(K25:N25), 0)</f>
         <v>0</v>
       </c>
@@ -4760,7 +4772,7 @@
       <c r="R28" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="S28" s="98">
+      <c r="S28" s="99">
         <f ca="1">VLOOKUP($T$12,$C$20:$P$25,13,FALSE)</f>
         <v>0</v>
       </c>
@@ -4793,12 +4805,12 @@
   </sheetData>
   <mergeCells count="50">
     <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C21:D21"/>
     <mergeCell ref="G24:H24"/>
-    <mergeCell ref="C21:D21"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="A11:B11"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C11:I11"/>
+    <mergeCell ref="A12:B25"/>
     <mergeCell ref="G23:H23"/>
     <mergeCell ref="R21:T21"/>
     <mergeCell ref="K12:P12"/>
@@ -4810,8 +4822,7 @@
     <mergeCell ref="M20:N20"/>
     <mergeCell ref="O20:P20"/>
     <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C11:I11"/>
-    <mergeCell ref="A12:B25"/>
+    <mergeCell ref="G20:H20"/>
     <mergeCell ref="S28:T28"/>
     <mergeCell ref="K22:L22"/>
     <mergeCell ref="M22:N22"/>
@@ -4826,7 +4837,7 @@
     <mergeCell ref="M24:N24"/>
     <mergeCell ref="K25:L25"/>
     <mergeCell ref="K24:L24"/>
-    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="O24:P24"/>
     <mergeCell ref="R11:T11"/>
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="M23:N23"/>
@@ -4842,6 +4853,7 @@
     <mergeCell ref="G21:H21"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E23:F23"/>
   </mergeCells>
   <conditionalFormatting sqref="T12">
     <cfRule type="cellIs" dxfId="154" priority="5" operator="equal">
@@ -6295,7 +6307,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -7029,10 +7041,12 @@
         <f>IFERROR(IF(INDEX('01.25'!D2:D500, MATCH(B25&amp;C25, INDEX('01.25'!B2:B500&amp;'01.25'!C2:C500, 0), 0))="", "", INDEX('01.25'!D2:D500, MATCH(B25&amp;C25, INDEX('01.25'!B2:B500&amp;'01.25'!C2:C500, 0), 0))), "")</f>
         <v>Ana Julia Pereira</v>
       </c>
-      <c r="E25" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" s="39"/>
+      <c r="E25" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="39" t="s">
+        <v>159</v>
+      </c>
       <c r="G25" s="48" t="s">
         <v>107</v>
       </c>
@@ -7119,7 +7133,7 @@
         <v>14</v>
       </c>
       <c r="F28" s="39" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G28" s="48" t="s">
         <v>107</v>
@@ -7274,7 +7288,7 @@
         <v>106</v>
       </c>
       <c r="K33" s="39" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -7295,7 +7309,7 @@
         <v>14</v>
       </c>
       <c r="F34" s="39" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G34" s="48" t="s">
         <v>107</v>
@@ -7383,7 +7397,7 @@
         <v>14</v>
       </c>
       <c r="F37" s="39" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G37" s="48" t="s">
         <v>107</v>
@@ -7441,7 +7455,7 @@
         <v>14</v>
       </c>
       <c r="F39" s="39" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G39" s="48" t="s">
         <v>107</v>
@@ -7587,7 +7601,7 @@
         <v>17</v>
       </c>
       <c r="F44" s="39" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G44" s="48" t="s">
         <v>107</v>
@@ -7673,7 +7687,7 @@
         <v>14</v>
       </c>
       <c r="F47" s="39" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G47" s="48" t="s">
         <v>107</v>
@@ -7848,7 +7862,7 @@
         <v>14</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G3" s="48" t="s">
         <v>107</v>
@@ -8050,7 +8064,7 @@
         <v>14</v>
       </c>
       <c r="F10" s="39" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G10" s="48" t="s">
         <v>107</v>
@@ -8080,7 +8094,7 @@
         <v>14</v>
       </c>
       <c r="F11" s="39" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="G11" s="48" t="s">
         <v>107</v>
@@ -8168,7 +8182,7 @@
         <v>14</v>
       </c>
       <c r="F14" s="39" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G14" s="48" t="s">
         <v>107</v>
@@ -8310,7 +8324,7 @@
         <v>14</v>
       </c>
       <c r="F19" s="39" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G19" s="48" t="s">
         <v>107</v>
@@ -8370,7 +8384,7 @@
         <v>14</v>
       </c>
       <c r="F21" s="39" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G21" s="48" t="s">
         <v>107</v>
@@ -8484,7 +8498,7 @@
         <v>14</v>
       </c>
       <c r="F25" s="39" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G25" s="48" t="s">
         <v>107</v>
@@ -8542,7 +8556,7 @@
         <v>14</v>
       </c>
       <c r="F27" s="39" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G27" s="48" t="s">
         <v>107</v>
@@ -8684,7 +8698,7 @@
         <v>14</v>
       </c>
       <c r="F32" s="39" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G32" s="48" t="s">
         <v>107</v>
@@ -8830,7 +8844,7 @@
         <v>14</v>
       </c>
       <c r="F37" s="39" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G37" s="48" t="s">
         <v>107</v>
@@ -8888,7 +8902,7 @@
         <v>14</v>
       </c>
       <c r="F39" s="39" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G39" s="48" t="s">
         <v>107</v>
@@ -8946,7 +8960,7 @@
         <v>14</v>
       </c>
       <c r="F41" s="39" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G41" s="48" t="s">
         <v>107</v>
@@ -9295,7 +9309,7 @@
         <v>14</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G3" s="48" t="s">
         <v>107</v>
@@ -9353,20 +9367,20 @@
         <v>14</v>
       </c>
       <c r="F5" s="39" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="G5" s="48" t="s">
         <v>107</v>
       </c>
       <c r="H5" s="39"/>
       <c r="I5" s="39" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="J5" s="39" t="s">
         <v>106</v>
       </c>
       <c r="K5" s="39" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -9387,7 +9401,7 @@
         <v>14</v>
       </c>
       <c r="F6" s="39" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G6" s="48" t="s">
         <v>107</v>
@@ -9417,7 +9431,7 @@
         <v>14</v>
       </c>
       <c r="F7" s="39" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G7" s="48" t="s">
         <v>107</v>
@@ -9531,7 +9545,7 @@
         <v>14</v>
       </c>
       <c r="F11" s="39" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G11" s="48" t="s">
         <v>107</v>
@@ -9561,7 +9575,7 @@
         <v>14</v>
       </c>
       <c r="F12" s="39" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G12" s="48" t="s">
         <v>107</v>
@@ -9619,7 +9633,7 @@
         <v>14</v>
       </c>
       <c r="F14" s="39" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G14" s="48" t="s">
         <v>107</v>
@@ -9649,7 +9663,7 @@
         <v>14</v>
       </c>
       <c r="F15" s="39" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G15" s="48" t="s">
         <v>107</v>
@@ -9765,7 +9779,7 @@
         <v>14</v>
       </c>
       <c r="F19" s="39" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="G19" s="48" t="s">
         <v>107</v>
@@ -9825,7 +9839,7 @@
         <v>14</v>
       </c>
       <c r="F21" s="39" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G21" s="48" t="s">
         <v>107</v>
@@ -9935,10 +9949,12 @@
         <f>IFERROR(IF(INDEX('01.25'!D2:D500, MATCH(B25&amp;C25, INDEX('01.25'!B2:B500&amp;'01.25'!C2:C500, 0), 0))="", "", INDEX('01.25'!D2:D500, MATCH(B25&amp;C25, INDEX('01.25'!B2:B500&amp;'01.25'!C2:C500, 0), 0))), "")</f>
         <v>Ana Julia Pereira</v>
       </c>
-      <c r="E25" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" s="39"/>
+      <c r="E25" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="39" t="s">
+        <v>159</v>
+      </c>
       <c r="G25" s="48" t="s">
         <v>107</v>
       </c>
@@ -9991,10 +10007,12 @@
         <f>IFERROR(IF(INDEX('01.25'!D2:D500, MATCH(B27&amp;C27, INDEX('01.25'!B2:B500&amp;'01.25'!C2:C500, 0), 0))="", "", INDEX('01.25'!D2:D500, MATCH(B27&amp;C27, INDEX('01.25'!B2:B500&amp;'01.25'!C2:C500, 0), 0))), "")</f>
         <v>Joao Lucas Côrtes Silva Freitas</v>
       </c>
-      <c r="E27" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27" s="39"/>
+      <c r="E27" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="39" t="s">
+        <v>180</v>
+      </c>
       <c r="G27" s="48" t="s">
         <v>107</v>
       </c>
@@ -10135,7 +10153,7 @@
         <v>14</v>
       </c>
       <c r="F32" s="39" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="G32" s="48" t="s">
         <v>107</v>
@@ -10165,7 +10183,7 @@
         <v>14</v>
       </c>
       <c r="F33" s="39" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G33" s="48" t="s">
         <v>107</v>
@@ -10195,7 +10213,7 @@
         <v>14</v>
       </c>
       <c r="F34" s="39" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G34" s="48" t="s">
         <v>107</v>
@@ -10337,7 +10355,7 @@
         <v>14</v>
       </c>
       <c r="F39" s="39" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G39" s="48" t="s">
         <v>107</v>
@@ -10451,7 +10469,7 @@
         <v>14</v>
       </c>
       <c r="F43" s="39" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="G43" s="48" t="s">
         <v>107</v>
@@ -10481,7 +10499,7 @@
         <v>14</v>
       </c>
       <c r="F44" s="39" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="G44" s="48" t="s">
         <v>107</v>
@@ -10567,7 +10585,7 @@
         <v>14</v>
       </c>
       <c r="F47" s="39" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="G47" s="48" t="s">
         <v>107</v>
@@ -10798,7 +10816,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="39" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="G5" s="48" t="s">
         <v>107</v>
@@ -10824,10 +10842,12 @@
         <f>IFERROR(IF(INDEX('01.25'!D2:D500, MATCH(B6&amp;C6, INDEX('01.25'!B2:B500&amp;'01.25'!C2:C500, 0), 0))="", "", INDEX('01.25'!D2:D500, MATCH(B6&amp;C6, INDEX('01.25'!B2:B500&amp;'01.25'!C2:C500, 0), 0))), "")</f>
         <v>Leonardo Zavilenski Fogaça</v>
       </c>
-      <c r="E6" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="39"/>
+      <c r="E6" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="39" t="s">
+        <v>159</v>
+      </c>
       <c r="G6" s="48" t="s">
         <v>107</v>
       </c>
@@ -10852,10 +10872,12 @@
         <f>IFERROR(IF(INDEX('01.25'!D2:D500, MATCH(B7&amp;C7, INDEX('01.25'!B2:B500&amp;'01.25'!C2:C500, 0), 0))="", "", INDEX('01.25'!D2:D500, MATCH(B7&amp;C7, INDEX('01.25'!B2:B500&amp;'01.25'!C2:C500, 0), 0))), "")</f>
         <v>Armindo Ferreira da Silva</v>
       </c>
-      <c r="E7" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="39"/>
+      <c r="E7" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="39" t="s">
+        <v>185</v>
+      </c>
       <c r="G7" s="48" t="s">
         <v>107</v>
       </c>
@@ -10964,10 +10986,12 @@
         <f>IFERROR(IF(INDEX('01.25'!D2:D500, MATCH(B11&amp;C11, INDEX('01.25'!B2:B500&amp;'01.25'!C2:C500, 0), 0))="", "", INDEX('01.25'!D2:D500, MATCH(B11&amp;C11, INDEX('01.25'!B2:B500&amp;'01.25'!C2:C500, 0), 0))), "")</f>
         <v>Analigia de Santana Abreu</v>
       </c>
-      <c r="E11" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="39"/>
+      <c r="E11" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="39" t="s">
+        <v>180</v>
+      </c>
       <c r="G11" s="48" t="s">
         <v>107</v>
       </c>
@@ -10996,7 +11020,7 @@
         <v>14</v>
       </c>
       <c r="F12" s="39" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="G12" s="48" t="s">
         <v>107</v>
@@ -11054,7 +11078,7 @@
         <v>14</v>
       </c>
       <c r="F14" s="39" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="G14" s="48" t="s">
         <v>107</v>
@@ -11196,7 +11220,7 @@
         <v>14</v>
       </c>
       <c r="F19" s="39" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="G19" s="48" t="s">
         <v>107</v>
@@ -11252,10 +11276,12 @@
         <f>IFERROR(IF(INDEX('01.25'!D2:D500, MATCH(B21&amp;C21, INDEX('01.25'!B2:B500&amp;'01.25'!C2:C500, 0), 0))="", "", INDEX('01.25'!D2:D500, MATCH(B21&amp;C21, INDEX('01.25'!B2:B500&amp;'01.25'!C2:C500, 0), 0))), "")</f>
         <v>Rony Eduardo Souza Terra</v>
       </c>
-      <c r="E21" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" s="39"/>
+      <c r="E21" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="39" t="s">
+        <v>188</v>
+      </c>
       <c r="G21" s="48" t="s">
         <v>107</v>
       </c>
@@ -11364,10 +11390,12 @@
         <f>IFERROR(IF(INDEX('01.25'!D2:D500, MATCH(B25&amp;C25, INDEX('01.25'!B2:B500&amp;'01.25'!C2:C500, 0), 0))="", "", INDEX('01.25'!D2:D500, MATCH(B25&amp;C25, INDEX('01.25'!B2:B500&amp;'01.25'!C2:C500, 0), 0))), "")</f>
         <v>Ana Julia Pereira</v>
       </c>
-      <c r="E25" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" s="39"/>
+      <c r="E25" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="39" t="s">
+        <v>189</v>
+      </c>
       <c r="G25" s="48" t="s">
         <v>107</v>
       </c>
@@ -11420,10 +11448,12 @@
         <f>IFERROR(IF(INDEX('01.25'!D2:D500, MATCH(B27&amp;C27, INDEX('01.25'!B2:B500&amp;'01.25'!C2:C500, 0), 0))="", "", INDEX('01.25'!D2:D500, MATCH(B27&amp;C27, INDEX('01.25'!B2:B500&amp;'01.25'!C2:C500, 0), 0))), "")</f>
         <v>Joao Lucas Côrtes Silva Freitas</v>
       </c>
-      <c r="E27" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" s="39"/>
+      <c r="E27" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="39" t="s">
+        <v>180</v>
+      </c>
       <c r="G27" s="48" t="s">
         <v>107</v>
       </c>
@@ -11588,10 +11618,12 @@
         <f>IFERROR(IF(INDEX('01.25'!D2:D500, MATCH(B33&amp;C33, INDEX('01.25'!B2:B500&amp;'01.25'!C2:C500, 0), 0))="", "", INDEX('01.25'!D2:D500, MATCH(B33&amp;C33, INDEX('01.25'!B2:B500&amp;'01.25'!C2:C500, 0), 0))), "")</f>
         <v>Vanessa Diovana Biassi Soares</v>
       </c>
-      <c r="E33" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="F33" s="39"/>
+      <c r="E33" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="39" t="s">
+        <v>159</v>
+      </c>
       <c r="G33" s="48" t="s">
         <v>107</v>
       </c>
@@ -11620,7 +11652,7 @@
         <v>14</v>
       </c>
       <c r="F34" s="39" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="G34" s="48" t="s">
         <v>107</v>
@@ -11902,7 +11934,7 @@
         <v>14</v>
       </c>
       <c r="F44" s="39" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="G44" s="48" t="s">
         <v>107</v>
@@ -13411,7 +13443,7 @@
         <v>99</v>
       </c>
       <c r="F1" s="37" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="G1" s="37" t="s">
         <v>100</v>
@@ -13423,7 +13455,7 @@
         <v>102</v>
       </c>
       <c r="J1" s="37" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="K1" s="37" t="s">
         <v>104</v>
@@ -13439,9 +13471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G5" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -16008,7 +16038,7 @@
         FALSE
     )
 )</f>
-        <v>Atrasado</v>
+        <v>Enviado</v>
       </c>
       <c r="O12" s="86" t="str">
         <f t="array" aca="1" ref="O12" ca="1">IF(
@@ -17592,7 +17622,7 @@
         FALSE
     )
 )</f>
-        <v>Atrasado &gt;= 2</v>
+        <v>Enviado</v>
       </c>
       <c r="L18" s="86" t="str">
         <f t="array" aca="1" ref="L18" ca="1">IF(
@@ -17636,7 +17666,7 @@
         FALSE
     )
 )</f>
-        <v>Atrasado &gt;= 2</v>
+        <v>Enviado</v>
       </c>
       <c r="N18" s="86" t="str">
         <f t="array" aca="1" ref="N18" ca="1">IF(
@@ -17658,7 +17688,7 @@
         FALSE
     )
 )</f>
-        <v>Atrasado</v>
+        <v>Enviado</v>
       </c>
       <c r="O18" s="86" t="str">
         <f t="array" aca="1" ref="O18" ca="1">IF(
@@ -18186,7 +18216,7 @@
         FALSE
     )
 )</f>
-        <v>Atrasado &gt;= 2</v>
+        <v>Enviado</v>
       </c>
       <c r="N20" s="86" t="str">
         <f t="array" aca="1" ref="N20" ca="1">IF(
@@ -18208,7 +18238,7 @@
         FALSE
     )
 )</f>
-        <v>Atrasado</v>
+        <v>Enviado</v>
       </c>
       <c r="O20" s="86" t="str">
         <f t="array" aca="1" ref="O20" ca="1">IF(
@@ -19633,7 +19663,7 @@
         FALSE
     )
 )</f>
-        <v>Atrasado</v>
+        <v>Enviado</v>
       </c>
       <c r="O27" s="86" t="str">
         <f t="array" aca="1" ref="O27" ca="1">IF(
@@ -19908,7 +19938,7 @@
         FALSE
     )
 )</f>
-        <v>Atrasado</v>
+        <v>Enviado</v>
       </c>
       <c r="O28" s="86" t="str">
         <f t="array" aca="1" ref="O28" ca="1">IF(
@@ -21008,7 +21038,7 @@
         FALSE
     )
 )</f>
-        <v>Atrasado</v>
+        <v>Enviado</v>
       </c>
       <c r="O32" s="86" t="str">
         <f t="array" aca="1" ref="O32" ca="1">IF(
@@ -21283,7 +21313,7 @@
         FALSE
     )
 )</f>
-        <v>Atrasado</v>
+        <v>Enviado</v>
       </c>
       <c r="O33" s="86" t="str">
         <f t="array" aca="1" ref="O33" ca="1">IF(

</xml_diff>